<commit_message>
Adding dynamic headers correction during row creation using template and hide column capability at style header and sheet level
</commit_message>
<xml_diff>
--- a/src/main/resources/excel/ExcelProcessorTestTemplate.xlsx
+++ b/src/main/resources/excel/ExcelProcessorTestTemplate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/salilvnair/workspace/git/salilvnair/excelprocessor/src/main/resources/excel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/salilvnair/Workspace/Personal/github/salilvnair/excelprocessor/src/main/resources/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1F86DED0-4267-6142-A343-C482BA51E540}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F374496F-08C8-944F-B132-221F26010866}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16680"/>
+    <workbookView xWindow="5560" yWindow="-18600" windowWidth="29400" windowHeight="16680" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="School" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="11">
   <si>
     <t>Name</t>
   </si>
@@ -63,12 +63,15 @@
   </si>
   <si>
     <t>Number of students</t>
+  </si>
+  <si>
+    <t>Testting</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -98,7 +101,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -121,14 +124,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -443,10 +458,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -494,11 +509,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -511,26 +526,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>2</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>